<commit_message>
feat: adds ukranian translation
</commit_message>
<xml_diff>
--- a/docassemble/ukraine/data/sources/interview_uk.xlsx
+++ b/docassemble/ukraine/data/sources/interview_uk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Desktop/tripliq-repo/docassemble-ukraine/docassemble/ukraine/data/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F122D9-9295-264B-8CB3-F4ACCC467FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AA830C-074E-1446-A8FB-08FCE114F33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23360" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15040" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="357">
   <si>
     <t>interview</t>
   </si>
@@ -1235,9 +1235,6 @@
     <t>Поточне місто проживання</t>
   </si>
   <si>
-    <t>Берлін</t>
-  </si>
-  <si>
     <t>Призначення резиденції</t>
   </si>
   <si>
@@ -1248,9 +1245,6 @@
   </si>
   <si>
     <t>Будь ласка, заповніть наступні запитання щодо вашого перебування в Німеччині</t>
-  </si>
-  <si>
-    <t>втеча від війни</t>
   </si>
   <si>
     <t>Майже готово, виконайте наведені нижче дії, перш ніж надсилати</t>
@@ -1697,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H126" sqref="H126"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4514,7 +4508,7 @@
         <v>232</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4566,7 +4560,7 @@
         <v>236</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>345</v>
+        <v>236</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4592,7 +4586,7 @@
         <v>238</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4618,7 +4612,7 @@
         <v>240</v>
       </c>
       <c r="H112" s="4" t="s">
-        <v>350</v>
+        <v>240</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4644,7 +4638,7 @@
         <v>242</v>
       </c>
       <c r="H113" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4696,7 +4690,7 @@
         <v>247</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4722,7 +4716,7 @@
         <v>249</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4748,7 +4742,7 @@
         <v>251</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4800,7 +4794,7 @@
         <v>255</v>
       </c>
       <c r="H119" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4826,7 +4820,7 @@
         <v>257</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4852,7 +4846,7 @@
         <v>261</v>
       </c>
       <c r="H121" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4878,7 +4872,7 @@
         <v>263</v>
       </c>
       <c r="H122" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.2">
@@ -4904,7 +4898,7 @@
         <v>265</v>
       </c>
       <c r="H123" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4956,7 +4950,7 @@
         <v>270</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: latest translation changes
</commit_message>
<xml_diff>
--- a/docassemble/ukraine/data/sources/interview_uk.xlsx
+++ b/docassemble/ukraine/data/sources/interview_uk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Desktop/tripliq-repo/docassemble-ukraine/docassemble/ukraine/data/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC4DD5A-6DEA-0842-8104-801F1374EF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAEAC87-34F1-6F4F-A85A-1B3B5A120AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,9 +409,6 @@
   </si>
   <si>
     <t>in eingetragener Lebenspartnerschaft lebend</t>
-  </si>
-  <si>
-    <t>проживання в зареєстрованому партнерстві</t>
   </si>
   <si>
     <t>6492c3801e8c049f5b8e6826b3d2b7d9</t>
@@ -1042,9 +1039,6 @@
   </si>
   <si>
     <t>Visum ausgestellt von</t>
-  </si>
-  <si>
-    <t>Віза видана</t>
   </si>
   <si>
     <t>d4908b1e39cc61772e5d74e5fb77d241</t>
@@ -1556,13 +1550,6 @@
     <t>зареєстрований у матері</t>
   </si>
   <si>
-    <t>TripliQ не включає ***юридичні консультації чи юридичниі послуги***, тобто не проводиться юридична експертиза конкретної окремої справи в рамках Закону про юридичні послуги (RDG) від TripliQ.
-- Ваші дані не зберігаються у нас довгостроково. Дані, які Ви вносите, використовуються лише для написання Вашої заяви. Після цього ваші дані будуть видалені.
-- Пропозиція «TripliQ»» підтримує клієнта за допомогою програмно-підтримуваного інтерв'ю та процесу створення договору при самостійному створенні його юридичних документів.
-– Цей процес в основному розроблений таким чином, що заявка не вимагає спеціальних юридичних знань. Однак автоматизований процес інтерв’ю не може охопити кожен факт з його специфічними характеристиками.
-- Тому замовник зобов'язаний піддати створені юридичні документи перевірці правдоподібності щодо цільового використання. У разі необхідності проведення юридичної експертизи в конкретному окремому випадку рекомендуємо звернутися за консультацією до юриста або іншого органу, уповноваженого надавати юридичні послуги відповідно до РДГ.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please choose your language.
 (Будь ласка, виберіть Вашу мову).
 Bitte wählen Sie eine Sprache aus.
@@ -1596,9 +1583,6 @@
     <t>Країна, в якій Ви народились</t>
   </si>
   <si>
-    <t>Чоловіча</t>
-  </si>
-  <si>
     <t>жіноча</t>
   </si>
   <si>
@@ -1617,9 +1601,6 @@
     <t>Національність</t>
   </si>
   <si>
-    <t>Попереднє громадянство вказати лише у випадку, якщо раніше у Вас було інше громадянство)</t>
-  </si>
-  <si>
     <t>Сімейний стан</t>
   </si>
   <si>
@@ -1650,9 +1631,6 @@
     <t>Прошу надати дозвіл на працевлаштування</t>
   </si>
   <si>
-    <t>Паспорт / посвідчення особи</t>
-  </si>
-  <si>
     <t>Будь ласка, заповніть паспортні дані чи інші дані, що посвідчують Вашу особу</t>
   </si>
   <si>
@@ -1666,9 +1644,6 @@
   </si>
   <si>
     <t>Видано в</t>
-  </si>
-  <si>
-    <t>Дійсний до</t>
   </si>
   <si>
     <t>Країна, в якій було видано документ</t>
@@ -1788,12 +1763,6 @@
 [Посилання на пошуковий сайт установ](https://bamf-navi.bamf.de/de/Themen/Behoerden/)
 &lt;br&gt;
 &lt;br&gt;</t>
-  </si>
-  <si>
-    <t>Записано правильну адресу з відео вище як адресу для заяви</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Зроблено копії усіх посвідчень/паспортів для прикріплення до заяви після її завантаження </t>
   </si>
   <si>
     <r>
@@ -1921,6 +1890,37 @@
   </si>
   <si>
     <t>військове біженство</t>
+  </si>
+  <si>
+    <t>TripliQ не включає *юридичні консультації чи юридичниі послуги*, тобто не проводиться юридична експертиза конкретної окремої справи в рамках Закону про юридичні послуги (RDG) від TripliQ.
+- Ваші дані не зберігаються у нас довгостроково. Дані, які Ви вносите, використовуються лише для написання Вашої заяви. Після цього ваші дані будуть видалені.
+- Пропозиція «TripliQ»» підтримує клієнта при самостійному створенні власних юридичних документів за допомогою процесу інтерв'ю та процесу створення договору на основі прогманого хабепечення.
+– Цей процес розроблений таким чином, що його використання не вимагає спеціальних юридичних знань. Однак автоматизований процес інтерв’ю не може охопити кожен окремий випадок з його особливостями.
+- Тому користувач зобов'язаний піддати створені юридичні документи перевірці правдоподібності щодо цільового використання. У разі необхідності проведення юридичної експертизи в конкретному окремому випадку рекомендуємо звернутися за консультацією до юриста або іншого органу, уповноваженого надавати юридичні послуги відповідно до Закону про юридичні послуги.</t>
+  </si>
+  <si>
+    <t>Попереднє громадянство (вказати лише у випадку, якщо раніше у Вас було інше громадянство)</t>
+  </si>
+  <si>
+    <t>проживаю в зареєстрованому партнерстві</t>
+  </si>
+  <si>
+    <t>чоловіча</t>
+  </si>
+  <si>
+    <t>Паспорт/ посвідчення особи</t>
+  </si>
+  <si>
+    <t>Дата видачі</t>
+  </si>
+  <si>
+    <t>Орган, що видав візу</t>
+  </si>
+  <si>
+    <t>Запишіть правильну адресу з відео вище, як адресу для заяви</t>
+  </si>
+  <si>
+    <t>Зробіть копії усіх посвідчень/паспортів для прикріплення до заяви після її завантаження</t>
   </si>
 </sst>
 </file>
@@ -2332,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E94" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2471,7 +2471,7 @@
         <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>392</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2627,7 +2627,7 @@
         <v>35</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2679,7 +2679,7 @@
         <v>39</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2705,7 +2705,7 @@
         <v>41</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2913,7 +2913,7 @@
         <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2965,7 +2965,7 @@
         <v>64</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3017,7 +3017,7 @@
         <v>69</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3043,7 +3043,7 @@
         <v>71</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3095,7 +3095,7 @@
         <v>75</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3147,7 +3147,7 @@
         <v>79</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3173,7 +3173,7 @@
         <v>81</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3251,7 +3251,7 @@
         <v>88</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>403</v>
+        <v>455</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3277,7 +3277,7 @@
         <v>90</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3303,7 +3303,7 @@
         <v>92</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3381,7 +3381,7 @@
         <v>100</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3407,7 +3407,7 @@
         <v>102</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3433,7 +3433,7 @@
         <v>104</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3459,7 +3459,7 @@
         <v>106</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -3485,7 +3485,7 @@
         <v>108</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>410</v>
+        <v>453</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3511,7 +3511,7 @@
         <v>110</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3537,7 +3537,7 @@
         <v>112</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3563,7 +3563,7 @@
         <v>114</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3589,7 +3589,7 @@
         <v>116</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3615,7 +3615,7 @@
         <v>118</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>119</v>
+        <v>454</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3629,19 +3629,19 @@
         <v>34</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="H50" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3655,19 +3655,19 @@
         <v>35</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="H51" s="4" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3681,19 +3681,19 @@
         <v>36</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H52" s="4" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3707,19 +3707,19 @@
         <v>37</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="H53" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3733,19 +3733,19 @@
         <v>38</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="H54" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3759,19 +3759,19 @@
         <v>39</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="H55" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3779,25 +3779,25 @@
         <v>8</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="H56" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3805,25 +3805,25 @@
         <v>8</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="H57" s="4" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3831,25 +3831,25 @@
         <v>8</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C58" s="2">
         <v>2</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="3" t="s">
+      <c r="H58" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3857,25 +3857,25 @@
         <v>8</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="H59" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3883,25 +3883,25 @@
         <v>8</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" s="2">
         <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="H60" s="4" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3909,25 +3909,25 @@
         <v>8</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C61" s="2">
         <v>2</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="H61" s="4" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3935,25 +3935,25 @@
         <v>8</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C62" s="2">
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="H62" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3961,25 +3961,25 @@
         <v>8</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C63" s="2">
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="H63" s="4" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3987,25 +3987,25 @@
         <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C64" s="2">
         <v>2</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="H64" s="4" t="s">
-        <v>421</v>
+        <v>456</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4013,25 +4013,25 @@
         <v>8</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" s="2">
         <v>3</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="H65" s="4" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4039,25 +4039,25 @@
         <v>8</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C66" s="2">
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="3" t="s">
+      <c r="H66" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="H66" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4065,25 +4065,25 @@
         <v>8</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C67" s="2">
         <v>5</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="H67" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4091,25 +4091,25 @@
         <v>8</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C68" s="2">
         <v>6</v>
       </c>
       <c r="D68" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="3" t="s">
+      <c r="H68" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4117,25 +4117,25 @@
         <v>8</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C69" s="2">
         <v>7</v>
       </c>
       <c r="D69" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="H69" s="4" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4143,25 +4143,25 @@
         <v>8</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C70" s="2">
         <v>8</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="H70" s="4" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4169,25 +4169,25 @@
         <v>8</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C71" s="2">
         <v>9</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="3" t="s">
+      <c r="H71" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4195,25 +4195,25 @@
         <v>8</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C72" s="2">
         <v>10</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H72" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4221,25 +4221,25 @@
         <v>8</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C73" s="2">
         <v>11</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="H73" s="4" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4247,25 +4247,25 @@
         <v>8</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C74" s="2">
         <v>12</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="H74" s="4" t="s">
-        <v>427</v>
+        <v>457</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4273,25 +4273,25 @@
         <v>8</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C75" s="2">
         <v>13</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="H75" s="4" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4299,25 +4299,25 @@
         <v>8</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="H76" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4325,25 +4325,25 @@
         <v>8</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="3" t="s">
+      <c r="H77" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -4351,25 +4351,25 @@
         <v>8</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C78" s="2">
         <v>2</v>
       </c>
       <c r="D78" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="H78" s="4" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4377,25 +4377,25 @@
         <v>8</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C79" s="2">
         <v>3</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="H79" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4403,22 +4403,22 @@
         <v>8</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C80" s="2">
         <v>4</v>
       </c>
       <c r="D80" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>65</v>
@@ -4429,25 +4429,25 @@
         <v>8</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C81" s="2">
         <v>5</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="H81" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4455,25 +4455,25 @@
         <v>8</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C82" s="2">
         <v>6</v>
       </c>
       <c r="D82" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="H82" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4481,25 +4481,25 @@
         <v>8</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C83" s="2">
         <v>7</v>
       </c>
       <c r="D83" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="H83" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4507,25 +4507,25 @@
         <v>8</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C84" s="2">
         <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="H84" s="4" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4533,25 +4533,25 @@
         <v>8</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C85" s="2">
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="H85" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4559,25 +4559,25 @@
         <v>8</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C86" s="2">
         <v>1</v>
       </c>
       <c r="D86" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>204</v>
-      </c>
       <c r="H86" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -4585,25 +4585,25 @@
         <v>8</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C87" s="2">
         <v>2</v>
       </c>
       <c r="D87" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="H87" s="4" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4611,25 +4611,25 @@
         <v>8</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C88" s="2">
         <v>3</v>
       </c>
       <c r="D88" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="H88" s="4" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4637,25 +4637,25 @@
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C89" s="2">
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="H89" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4663,25 +4663,25 @@
         <v>8</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C90" s="2">
         <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="H90" s="4" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4689,25 +4689,25 @@
         <v>8</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C91" s="2">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="H91" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4715,25 +4715,25 @@
         <v>8</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C92" s="2">
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="H92" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4741,25 +4741,25 @@
         <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C93" s="2">
         <v>2</v>
       </c>
       <c r="D93" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="H93" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4767,25 +4767,25 @@
         <v>8</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C94" s="2">
         <v>3</v>
       </c>
       <c r="D94" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="H94" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4793,25 +4793,25 @@
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C95" s="2">
         <v>4</v>
       </c>
       <c r="D95" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G95" s="3" t="s">
+      <c r="H95" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="H95" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4819,25 +4819,25 @@
         <v>8</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C96" s="2">
         <v>5</v>
       </c>
       <c r="D96" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G96" s="3" t="s">
+      <c r="H96" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="H96" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4845,25 +4845,25 @@
         <v>8</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C97" s="2">
         <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G97" s="3" t="s">
+      <c r="H97" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="H97" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4871,25 +4871,25 @@
         <v>8</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C98" s="2">
         <v>7</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G98" s="3" t="s">
+      <c r="H98" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="H98" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4897,25 +4897,25 @@
         <v>8</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C99" s="2">
         <v>8</v>
       </c>
       <c r="D99" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="H99" s="4" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4923,25 +4923,25 @@
         <v>8</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C100" s="2">
         <v>9</v>
       </c>
       <c r="D100" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G100" s="3" t="s">
+      <c r="H100" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4949,25 +4949,25 @@
         <v>8</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C101" s="2">
         <v>10</v>
       </c>
       <c r="D101" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G101" s="3" t="s">
+      <c r="H101" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4975,25 +4975,25 @@
         <v>8</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C102" s="2">
         <v>11</v>
       </c>
       <c r="D102" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>244</v>
-      </c>
       <c r="H102" s="4" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5001,25 +5001,25 @@
         <v>8</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C103" s="2">
         <v>12</v>
       </c>
       <c r="D103" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G103" s="3" t="s">
+      <c r="H103" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="H103" s="4" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5027,25 +5027,25 @@
         <v>8</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C104" s="2">
         <v>13</v>
       </c>
       <c r="D104" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" s="3" t="s">
+      <c r="H104" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="H104" s="4" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5053,25 +5053,25 @@
         <v>8</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C105" s="2">
         <v>14</v>
       </c>
       <c r="D105" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="3" t="s">
+      <c r="H105" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="H105" s="4" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5079,25 +5079,25 @@
         <v>8</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C106" s="2">
         <v>15</v>
       </c>
       <c r="D106" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G106" s="3" t="s">
+      <c r="H106" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="H106" s="4" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5105,25 +5105,25 @@
         <v>8</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C107" s="2">
         <v>16</v>
       </c>
       <c r="D107" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>258</v>
-      </c>
       <c r="H107" s="4" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5131,25 +5131,25 @@
         <v>8</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C108" s="2">
         <v>17</v>
       </c>
       <c r="D108" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>261</v>
-      </c>
       <c r="H108" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5157,25 +5157,25 @@
         <v>8</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="H109" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5183,25 +5183,25 @@
         <v>8</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C110" s="2">
         <v>1</v>
       </c>
       <c r="D110" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>266</v>
-      </c>
       <c r="H110" s="4" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5209,25 +5209,25 @@
         <v>8</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="H111" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5235,25 +5235,25 @@
         <v>8</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C112" s="2">
         <v>1</v>
       </c>
       <c r="D112" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="3" t="s">
+      <c r="H112" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5261,25 +5261,25 @@
         <v>8</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C113" s="2">
         <v>2</v>
       </c>
       <c r="D113" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>274</v>
-      </c>
       <c r="H113" s="4" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5287,25 +5287,25 @@
         <v>8</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C114" s="2">
         <v>3</v>
       </c>
       <c r="D114" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="3" t="s">
+      <c r="H114" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="H114" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5313,25 +5313,25 @@
         <v>8</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C115" s="2">
         <v>4</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="H115" s="4" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5339,25 +5339,25 @@
         <v>8</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C116" s="2">
         <v>5</v>
       </c>
       <c r="D116" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="3" t="s">
+      <c r="H116" s="4" t="s">
         <v>281</v>
-      </c>
-      <c r="H116" s="4" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5365,25 +5365,25 @@
         <v>8</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C117" s="2">
         <v>6</v>
       </c>
       <c r="D117" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G117" s="3" t="s">
+      <c r="H117" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="H117" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5391,25 +5391,25 @@
         <v>8</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C118" s="2">
         <v>7</v>
       </c>
       <c r="D118" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G118" s="3" t="s">
+      <c r="H118" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="H118" s="4" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5417,25 +5417,25 @@
         <v>8</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C119" s="2">
         <v>8</v>
       </c>
       <c r="D119" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E119" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="H119" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5443,25 +5443,25 @@
         <v>8</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C120" s="2">
         <v>9</v>
       </c>
       <c r="D120" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G120" s="3" t="s">
+      <c r="H120" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="H120" s="4" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5469,25 +5469,25 @@
         <v>8</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C121" s="2">
         <v>10</v>
       </c>
       <c r="D121" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G121" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G121" s="3" t="s">
+      <c r="H121" s="4" t="s">
         <v>295</v>
-      </c>
-      <c r="H121" s="4" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5495,25 +5495,25 @@
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C122" s="2">
         <v>11</v>
       </c>
       <c r="D122" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E122" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="H122" s="4" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5521,25 +5521,25 @@
         <v>8</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C123" s="2">
         <v>12</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G123" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G123" s="3" t="s">
+      <c r="H123" s="4" t="s">
         <v>300</v>
-      </c>
-      <c r="H123" s="4" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5547,25 +5547,25 @@
         <v>8</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C124" s="2">
         <v>13</v>
       </c>
       <c r="D124" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G124" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E124" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G124" s="3" t="s">
+      <c r="H124" s="4" t="s">
         <v>303</v>
-      </c>
-      <c r="H124" s="4" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5573,25 +5573,25 @@
         <v>8</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C125" s="2">
         <v>14</v>
       </c>
       <c r="D125" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G125" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>306</v>
-      </c>
       <c r="H125" s="4" t="s">
-        <v>307</v>
+        <v>458</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5599,13 +5599,13 @@
         <v>8</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C126" s="2">
         <v>15</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>11</v>
@@ -5614,10 +5614,10 @@
         <v>12</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H126" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5625,25 +5625,25 @@
         <v>8</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C127" s="2">
         <v>16</v>
       </c>
       <c r="D127" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H127" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="H127" s="4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5651,25 +5651,25 @@
         <v>8</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C128" s="2">
         <v>17</v>
       </c>
       <c r="D128" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H128" s="4" t="s">
         <v>313</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H128" s="4" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5677,25 +5677,25 @@
         <v>8</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C129" s="2">
         <v>18</v>
       </c>
       <c r="D129" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H129" s="4" t="s">
         <v>316</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="H129" s="4" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5703,13 +5703,13 @@
         <v>8</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C130" s="2">
         <v>19</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>11</v>
@@ -5718,10 +5718,10 @@
         <v>12</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H130" s="4" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5729,13 +5729,13 @@
         <v>8</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C131" s="2">
         <v>20</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>11</v>
@@ -5744,10 +5744,10 @@
         <v>12</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H131" s="4" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5755,13 +5755,13 @@
         <v>8</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C132" s="2">
         <v>21</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>11</v>
@@ -5770,10 +5770,10 @@
         <v>12</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H132" s="4" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5781,13 +5781,13 @@
         <v>8</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C133" s="2">
         <v>0</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>11</v>
@@ -5796,10 +5796,10 @@
         <v>12</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H133" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5807,25 +5807,25 @@
         <v>8</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C134" s="2">
         <v>1</v>
       </c>
       <c r="D134" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="H134" s="4" t="s">
         <v>328</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G134" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="H134" s="4" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5833,25 +5833,25 @@
         <v>8</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C135" s="2">
         <v>2</v>
       </c>
       <c r="D135" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="H135" s="4" t="s">
         <v>331</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G135" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H135" s="4" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5859,13 +5859,13 @@
         <v>8</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C136" s="2">
         <v>3</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>11</v>
@@ -5874,10 +5874,10 @@
         <v>12</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H136" s="4" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5885,13 +5885,13 @@
         <v>8</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C137" s="2">
         <v>4</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>11</v>
@@ -5900,10 +5900,10 @@
         <v>12</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H137" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5911,25 +5911,25 @@
         <v>8</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C138" s="2">
         <v>5</v>
       </c>
       <c r="D138" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H138" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="H138" s="4" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5937,13 +5937,13 @@
         <v>8</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C139" s="2">
         <v>6</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>11</v>
@@ -5952,10 +5952,10 @@
         <v>12</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H139" s="4" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5963,13 +5963,13 @@
         <v>8</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C140" s="2">
         <v>7</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>11</v>
@@ -5978,10 +5978,10 @@
         <v>12</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H140" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5989,13 +5989,13 @@
         <v>8</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C141" s="2">
         <v>8</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>11</v>
@@ -6004,10 +6004,10 @@
         <v>12</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H141" s="4" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6015,13 +6015,13 @@
         <v>8</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C142" s="2">
         <v>9</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>11</v>
@@ -6030,10 +6030,10 @@
         <v>12</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H142" s="4" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6041,13 +6041,13 @@
         <v>8</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C143" s="2">
         <v>10</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>11</v>
@@ -6056,10 +6056,10 @@
         <v>12</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H143" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6067,25 +6067,25 @@
         <v>8</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C144" s="2">
         <v>11</v>
       </c>
       <c r="D144" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H144" s="4" t="s">
         <v>351</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G144" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H144" s="4" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6093,13 +6093,13 @@
         <v>8</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>11</v>
@@ -6108,10 +6108,10 @@
         <v>12</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H145" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6119,13 +6119,13 @@
         <v>8</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C146" s="2">
         <v>1</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>11</v>
@@ -6134,10 +6134,10 @@
         <v>12</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H146" s="4" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -6145,13 +6145,13 @@
         <v>8</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C147" s="2">
         <v>2</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>11</v>
@@ -6160,10 +6160,10 @@
         <v>12</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H147" s="4" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6171,13 +6171,13 @@
         <v>8</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C148" s="2">
         <v>3</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>11</v>
@@ -6186,10 +6186,10 @@
         <v>12</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H148" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6197,13 +6197,13 @@
         <v>8</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C149" s="2">
         <v>4</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>11</v>
@@ -6212,10 +6212,10 @@
         <v>12</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6223,13 +6223,13 @@
         <v>8</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C150" s="2">
         <v>5</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>11</v>
@@ -6238,24 +6238,24 @@
         <v>12</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H150" s="4" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>11</v>
@@ -6264,50 +6264,50 @@
         <v>12</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H151" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C152" s="2">
         <v>1</v>
       </c>
       <c r="D152" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="H152" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G152" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="H152" s="4" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C153" s="2">
         <v>2</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>11</v>
@@ -6316,50 +6316,50 @@
         <v>12</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H153" s="4" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
       </c>
       <c r="D154" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H154" s="4" t="s">
         <v>377</v>
-      </c>
-      <c r="E154" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F154" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G154" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="H154" s="4" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C155" s="2">
         <v>1</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>11</v>
@@ -6368,7 +6368,7 @@
         <v>12</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H155" s="4" t="s">
         <v>26</v>
@@ -6379,13 +6379,13 @@
         <v>8</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C156" s="2">
         <v>1021</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>11</v>
@@ -6394,10 +6394,10 @@
         <v>12</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H156" s="4" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6411,19 +6411,19 @@
         <v>1023</v>
       </c>
       <c r="D157" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="H157" s="4" t="s">
         <v>384</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G157" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="H157" s="4" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -6431,13 +6431,13 @@
         <v>8</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C158" s="2">
         <v>1002</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>11</v>
@@ -6446,10 +6446,10 @@
         <v>12</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H158" s="4" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6457,13 +6457,13 @@
         <v>8</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C159" s="2">
         <v>1002</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>11</v>
@@ -6472,10 +6472,10 @@
         <v>12</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H159" s="4" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>